<commit_message>
docs: added infixed tree traversal algoritm section to the document_conception.docx
</commit_message>
<xml_diff>
--- a/docs/EnCours/Sprint1c - Outil de planification.xlsx
+++ b/docs/EnCours/Sprint1c - Outil de planification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remsc\OneDrive\Desktop\GIT\KitchenCompanion\docs\EnCours\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julienc./Desktop/KitchenCompanion/docs/EnCours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782B70FB-4CD9-483D-BAC2-470E2DD1D0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99A37C0-10DF-1545-AA44-242F9A37E3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="24900" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planification" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -117,7 +117,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -126,13 +126,51 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Cette colonne sert à déclarer et nommer chacune des tâches importantes à réaliser. Chaque nom doit être concis et précis.
-Optionnellement, il est possible d'ajouter une note donnant des l'informations complémentaires. L'objectif étant de clarifier et désambigüer les détails techniques de la tâche.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Cette colonne sert à déclarer et nommer chacune des tâches importantes à réaliser. Chaque nom doit être concis et précis.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optionnellement, il est possible d'ajouter une note donnant des l'informations complémentaires. L'objectif étant de clarifier et désambigüer les détails techniques de la tâche.</t>
         </r>
       </text>
     </comment>
@@ -142,23 +180,71 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Dépendance</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dépendance</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-La notion de dépendance fait référence au fait qu'une tâche dépend d'une autre.
-L'identification d'une telle dépendance permet d'identifier l'ordre de développement.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">La notion de dépendance fait référence au fait qu'une tâche dépend d'une autre.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>L'identification d'une telle dépendance permet d'identifier l'ordre de développement.</t>
         </r>
       </text>
     </comment>
@@ -383,7 +469,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="107">
   <si>
     <t>Planification</t>
   </si>
@@ -717,6 +803,120 @@
   <si>
     <t>Rédaction du document de définition</t>
   </si>
+  <si>
+    <t>Julien</t>
+  </si>
+  <si>
+    <t>Coulombe-Morency</t>
+  </si>
+  <si>
+    <t>Rémi</t>
+  </si>
+  <si>
+    <t>Chuet</t>
+  </si>
+  <si>
+    <t>Création du serveur Next.js</t>
+  </si>
+  <si>
+    <t>Création de la base de donnée Prisma</t>
+  </si>
+  <si>
+    <t>Ajout:  Module d'authentification -  Changer le type de compte utilisateur (Membre vers Chef)</t>
+  </si>
+  <si>
+    <t>Implémentation: Module d'authentification</t>
+  </si>
+  <si>
+    <t>Implémentation: DAO</t>
+  </si>
+  <si>
+    <t>Fonctionalité: Création des comptes usager administrateur</t>
+  </si>
+  <si>
+    <t>Implémentation: Module - Liste de prix (fournisseur, non modifiable)</t>
+  </si>
+  <si>
+    <t>Implémentation: Module - Liste de prix (marché, modifiable)</t>
+  </si>
+  <si>
+    <t>Implémentation:  Stratégie -  Conversion d'unité de mesure</t>
+  </si>
+  <si>
+    <t>Implémentation: Module de gestion de recettes</t>
+  </si>
+  <si>
+    <t>Implémentation:  Logique du Composite de Menu,Recette,Ingrédients</t>
+  </si>
+  <si>
+    <t>Implémentation : Livres de recettes</t>
+  </si>
+  <si>
+    <t>Fonctionnalité : Ajout et de modification de recettes</t>
+  </si>
+  <si>
+    <t>Implémentation : Module de gestion des menus</t>
+  </si>
+  <si>
+    <t>Algoritme: Calcul du coût de reviens dans la structure Composite</t>
+  </si>
+  <si>
+    <t>Fonctionalité: Créer des usager de type membre</t>
+  </si>
+  <si>
+    <t>Implémentation: Module de gestion des brigades</t>
+  </si>
+  <si>
+    <t>Implémentation: Options de partages de menus</t>
+  </si>
+  <si>
+    <t>Initialisation du projet (package.json, typescript.config, github test)</t>
+  </si>
+  <si>
+    <t>Implémentation: Module registre MAPAQ</t>
+  </si>
+  <si>
+    <t>Fonctionalité: Alerte températures trop haute</t>
+  </si>
+  <si>
+    <t>Fonctionalité: Ajouter des températures au registre</t>
+  </si>
+  <si>
+    <t>Fonctionalité: Création de frigo</t>
+  </si>
+  <si>
+    <t>Fonctionnalité: Notification (modification d'un menu)</t>
+  </si>
+  <si>
+    <t>Implémentation: Module de gestion de contacts</t>
+  </si>
+  <si>
+    <t>Implémentation: Façade CréationPDF</t>
+  </si>
+  <si>
+    <t>Fonctionalité: Exportation des recettes, menu, livre de recettes, liste d'ingrédients</t>
+  </si>
+  <si>
+    <t>Fonctionalité: Tutoriel intéractif</t>
+  </si>
+  <si>
+    <t>Fonctionalité: Gestion des médias (video, avatar, image recette)</t>
+  </si>
+  <si>
+    <t>Implémentation: Création et destruction de membres et rôle dans une brigade</t>
+  </si>
+  <si>
+    <t>Implémentation: Gestion du compte utilisateur (mot de passe, nom, etc.)</t>
+  </si>
+  <si>
+    <t>Implémentation: Internationalisation (ajout des version anglaise à la base de donnée)</t>
+  </si>
+  <si>
+    <t>Déploiement</t>
+  </si>
+  <si>
+    <t>00.15</t>
+  </si>
 </sst>
 </file>
 
@@ -725,7 +925,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -839,6 +1039,19 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1280,7 +1493,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1342,7 +1555,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1533,7 +1746,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1654,7 +1867,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1688,7 +1901,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1702,7 +1915,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1764,7 +1977,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1826,7 +2039,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1943,7 +2156,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -2060,7 +2273,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -2179,7 +2392,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -2300,7 +2513,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="671525696"/>
@@ -2359,7 +2572,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="671528216"/>
@@ -2401,7 +2614,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2435,7 +2648,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2449,7 +2662,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2511,7 +2724,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2567,10 +2780,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>4</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3229166666653667</c:v>
+                  <c:v>6.4062499999970894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2626,10 +2839,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.20833333333333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2753,7 +2966,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="588507136"/>
@@ -2812,7 +3025,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="588508216"/>
@@ -2854,7 +3067,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2888,7 +3101,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2902,7 +3115,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2964,7 +3177,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3020,10 +3233,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2916666666666671E-2</c:v>
+                  <c:v>1.6979166666667314</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3079,10 +3292,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>1.2083333333332149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3138,10 +3351,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99999999999870004</c:v>
+                  <c:v>3.7083333333304758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3206,7 +3419,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="671530016"/>
@@ -3265,7 +3478,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="671533256"/>
@@ -3307,7 +3520,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3341,7 +3554,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3355,7 +3568,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3417,7 +3630,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3473,10 +3686,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>3</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32291666666666669</c:v>
+                  <c:v>2.2812500000000635</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3532,10 +3745,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99999999999870004</c:v>
+                  <c:v>2.874999999997403</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3591,10 +3804,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.458333333332956</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3659,7 +3872,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="473329656"/>
@@ -3718,7 +3931,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="473329296"/>
@@ -3760,7 +3973,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3794,7 +4007,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7366,28 +7579,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AF97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:G24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C16" zoomScale="178" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="0.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="0.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" style="1" customWidth="1"/>
     <col min="4" max="5" width="19" style="1" customWidth="1"/>
-    <col min="6" max="7" width="11.6328125" style="1" customWidth="1"/>
-    <col min="8" max="14" width="8.54296875" style="2" customWidth="1"/>
-    <col min="15" max="18" width="9.26953125" style="1"/>
+    <col min="6" max="7" width="11.6640625" style="1" customWidth="1"/>
+    <col min="8" max="14" width="8.5" style="2" customWidth="1"/>
+    <col min="15" max="18" width="9.33203125" style="1"/>
     <col min="19" max="19" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="20" max="21" width="9.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="22" max="27" width="9.26953125" style="2" hidden="1" customWidth="1"/>
-    <col min="28" max="32" width="9.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.26953125" style="1"/>
+    <col min="20" max="21" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="22" max="27" width="9.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="28" max="32" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" ht="12.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:31" ht="25.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:31" ht="13" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:31" ht="25.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B2" s="17"/>
       <c r="C2" s="44" t="s">
         <v>9</v>
@@ -7404,7 +7617,7 @@
       <c r="M2" s="44"/>
       <c r="N2" s="44"/>
     </row>
-    <row r="3" spans="2:31" ht="12.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:31" ht="13" thickTop="1" x14ac:dyDescent="0.15">
       <c r="C3" s="45" t="s">
         <v>27</v>
       </c>
@@ -7420,8 +7633,8 @@
       <c r="M3" s="45"/>
       <c r="N3" s="45"/>
     </row>
-    <row r="4" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:31" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="5" spans="2:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18"/>
       <c r="C5" s="46" t="s">
         <v>47</v>
@@ -7438,14 +7651,14 @@
       <c r="M5" s="46"/>
       <c r="N5" s="46"/>
     </row>
-    <row r="6" spans="2:31" ht="6.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:31" ht="6.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="I6" s="15"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="2:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C7" s="5"/>
       <c r="D7" s="16" t="s">
         <v>2</v>
@@ -7467,31 +7680,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:31" x14ac:dyDescent="0.15">
       <c r="C8" s="8">
         <v>1</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="D8" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>70</v>
+      </c>
       <c r="F8" s="8" t="str">
         <f>IF(C8&lt;=$N$7,UPPER(LEFT(D8)) &amp; UPPER(LEFT(E8)),"")</f>
-        <v/>
+        <v>JC</v>
       </c>
       <c r="I8" s="15"/>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:31" x14ac:dyDescent="0.15">
       <c r="C9" s="7">
         <v>2</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
+      <c r="D9" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>72</v>
+      </c>
       <c r="F9" s="7" t="str">
         <f t="shared" ref="F9:F11" si="0">IF(C9&lt;=$N$7,UPPER(LEFT(D9)) &amp; UPPER(LEFT(E9)),"")</f>
-        <v/>
+        <v>RC</v>
       </c>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.15">
       <c r="C10" s="8">
         <v>3</v>
       </c>
@@ -7503,7 +7724,7 @@
       </c>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.15">
       <c r="C11" s="7">
         <v>4</v>
       </c>
@@ -7514,8 +7735,8 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:31" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="2:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="46" t="s">
         <v>0</v>
@@ -7533,15 +7754,15 @@
       <c r="N13" s="46"/>
       <c r="U13" s="2">
         <f>D68</f>
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="AA13" s="2">
         <f>N7</f>
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:31" ht="6.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="2:31" s="4" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:31" ht="6.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="2:31" s="4" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
         <v>3</v>
       </c>
@@ -7597,7 +7818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:31" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:31" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C16" s="11">
         <v>1</v>
       </c>
@@ -7641,7 +7862,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C17" s="12">
         <v>2</v>
       </c>
@@ -7710,7 +7931,7 @@
         <v>1.3229166666653667</v>
       </c>
     </row>
-    <row r="18" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C18" s="13">
         <v>3</v>
       </c>
@@ -7765,7 +7986,7 @@
       </c>
       <c r="AA18" s="2" t="str">
         <f>F8</f>
-        <v/>
+        <v>JC</v>
       </c>
       <c r="AB18" s="1">
         <v>1</v>
@@ -7783,7 +8004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C19" s="12">
         <v>4</v>
       </c>
@@ -7838,7 +8059,7 @@
       </c>
       <c r="AA19" s="2" t="str">
         <f>F9</f>
-        <v/>
+        <v>RC</v>
       </c>
       <c r="AB19" s="1">
         <v>2</v>
@@ -7856,24 +8077,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C20" s="13">
         <v>5</v>
       </c>
-      <c r="D20" s="39"/>
+      <c r="D20" s="39" t="s">
+        <v>91</v>
+      </c>
       <c r="E20" s="39"/>
       <c r="F20" s="39"/>
       <c r="G20" s="39"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="35"/>
+      <c r="H20" s="34">
+        <v>2</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="34">
+        <v>1</v>
+      </c>
+      <c r="K20" s="34">
+        <v>1</v>
+      </c>
+      <c r="L20" s="35">
+        <v>4.1666666666666699E-2</v>
+      </c>
       <c r="M20" s="34"/>
       <c r="N20" s="34"/>
       <c r="T20" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U20" s="2">
         <v>4</v>
@@ -7901,24 +8134,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C21" s="12">
         <v>6</v>
       </c>
-      <c r="D21" s="42"/>
+      <c r="D21" s="42" t="s">
+        <v>73</v>
+      </c>
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
       <c r="G21" s="42"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="33"/>
+      <c r="H21" s="32">
+        <v>5</v>
+      </c>
+      <c r="I21" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="32">
+        <v>1</v>
+      </c>
+      <c r="K21" s="32">
+        <v>1</v>
+      </c>
+      <c r="L21" s="33" t="s">
+        <v>106</v>
+      </c>
       <c r="M21" s="32"/>
       <c r="N21" s="32"/>
       <c r="T21" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21" s="2">
         <v>5</v>
@@ -7931,24 +8176,36 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C22" s="13">
         <v>7</v>
       </c>
-      <c r="D22" s="39"/>
+      <c r="D22" s="39" t="s">
+        <v>74</v>
+      </c>
       <c r="E22" s="39"/>
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="35"/>
+      <c r="H22" s="34">
+        <v>5</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="34">
+        <v>2</v>
+      </c>
+      <c r="K22" s="34">
+        <v>1</v>
+      </c>
+      <c r="L22" s="35">
+        <v>0.16666666666666599</v>
+      </c>
       <c r="M22" s="34"/>
       <c r="N22" s="34"/>
       <c r="T22" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22" s="2">
         <v>6</v>
@@ -7957,24 +8214,36 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="23" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C23" s="12">
         <v>8</v>
       </c>
-      <c r="D23" s="42"/>
+      <c r="D23" s="42" t="s">
+        <v>77</v>
+      </c>
       <c r="E23" s="42"/>
       <c r="F23" s="42"/>
       <c r="G23" s="42"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="33"/>
+      <c r="H23" s="32">
+        <v>7</v>
+      </c>
+      <c r="I23" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="32">
+        <v>2</v>
+      </c>
+      <c r="K23" s="32">
+        <v>1</v>
+      </c>
+      <c r="L23" s="33">
+        <v>0.16666666666666599</v>
+      </c>
       <c r="M23" s="32"/>
       <c r="N23" s="32"/>
       <c r="T23" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" s="2">
         <v>7</v>
@@ -7992,24 +8261,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C24" s="13">
         <v>9</v>
       </c>
-      <c r="D24" s="39"/>
+      <c r="D24" s="39" t="s">
+        <v>76</v>
+      </c>
       <c r="E24" s="39"/>
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="35"/>
+      <c r="H24" s="34">
+        <v>7</v>
+      </c>
+      <c r="I24" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="34">
+        <v>3</v>
+      </c>
+      <c r="K24" s="34">
+        <v>2</v>
+      </c>
+      <c r="L24" s="35">
+        <v>0.250000000000003</v>
+      </c>
       <c r="M24" s="34"/>
       <c r="N24" s="34"/>
       <c r="T24" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U24" s="2">
         <v>8</v>
@@ -8030,24 +8311,36 @@
         <v>1.3229166666653667</v>
       </c>
     </row>
-    <row r="25" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C25" s="12">
         <v>10</v>
       </c>
-      <c r="D25" s="42"/>
+      <c r="D25" s="42" t="s">
+        <v>78</v>
+      </c>
       <c r="E25" s="42"/>
       <c r="F25" s="42"/>
       <c r="G25" s="42"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="33"/>
+      <c r="H25" s="32">
+        <v>9</v>
+      </c>
+      <c r="I25" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="32">
+        <v>1</v>
+      </c>
+      <c r="K25" s="32">
+        <v>1</v>
+      </c>
+      <c r="L25" s="33">
+        <v>4.1666666666666699E-2</v>
+      </c>
       <c r="M25" s="32"/>
       <c r="N25" s="32"/>
       <c r="T25" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>ISBLANK(D25)</f>
+        <v>0</v>
       </c>
       <c r="U25" s="2">
         <v>9</v>
@@ -8057,35 +8350,47 @@
       </c>
       <c r="AC25" s="1" t="str">
         <f t="shared" ref="AC25:AC28" si="3">AA18</f>
-        <v/>
+        <v>JC</v>
       </c>
       <c r="AD25" s="1">
         <f>COUNTIF(Responsabilite,AC25)</f>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="AE25" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC25)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C26" s="13">
         <v>11</v>
       </c>
-      <c r="D26" s="39"/>
+      <c r="D26" s="39" t="s">
+        <v>79</v>
+      </c>
       <c r="E26" s="39"/>
       <c r="F26" s="39"/>
       <c r="G26" s="39"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="35"/>
+      <c r="H26" s="34">
+        <v>7</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="34">
+        <v>3</v>
+      </c>
+      <c r="K26" s="34">
+        <v>2</v>
+      </c>
+      <c r="L26" s="35">
+        <v>0.625</v>
+      </c>
       <c r="M26" s="34"/>
       <c r="N26" s="34"/>
       <c r="T26" s="1" t="b">
         <f>ISBLANK(D26)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U26" s="2">
         <v>10</v>
@@ -8095,35 +8400,47 @@
       </c>
       <c r="AC26" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>RC</v>
       </c>
       <c r="AD26" s="1">
         <f>COUNTIF(Responsabilite,AC26)</f>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="AE26" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C27" s="12">
         <v>12</v>
       </c>
-      <c r="D27" s="42"/>
+      <c r="D27" s="42" t="s">
+        <v>80</v>
+      </c>
       <c r="E27" s="42"/>
       <c r="F27" s="42"/>
       <c r="G27" s="42"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="33"/>
+      <c r="H27" s="32">
+        <v>7</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="32">
+        <v>1</v>
+      </c>
+      <c r="K27" s="32">
+        <v>1</v>
+      </c>
+      <c r="L27" s="33">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="M27" s="32"/>
       <c r="N27" s="32"/>
       <c r="T27" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>ISBLANK(D27)</f>
+        <v>0</v>
       </c>
       <c r="U27" s="2">
         <v>11</v>
@@ -8141,27 +8458,39 @@
       </c>
       <c r="AE27" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC27)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:31" x14ac:dyDescent="0.3">
+        <v>5.2916666666650558</v>
+      </c>
+    </row>
+    <row r="28" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C28" s="13">
         <v>13</v>
       </c>
-      <c r="D28" s="39"/>
+      <c r="D28" s="39" t="s">
+        <v>81</v>
+      </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
       <c r="G28" s="39"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="35"/>
+      <c r="H28" s="34">
+        <v>7</v>
+      </c>
+      <c r="I28" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="34">
+        <v>1</v>
+      </c>
+      <c r="K28" s="34">
+        <v>1</v>
+      </c>
+      <c r="L28" s="35">
+        <v>0.250000000000003</v>
+      </c>
       <c r="M28" s="34"/>
       <c r="N28" s="34"/>
       <c r="T28" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>ISBLANK(D28)</f>
+        <v>0</v>
       </c>
       <c r="U28" s="2">
         <v>12</v>
@@ -8179,27 +8508,39 @@
       </c>
       <c r="AE28" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="3:31" x14ac:dyDescent="0.3">
+        <v>5.2916666666650558</v>
+      </c>
+    </row>
+    <row r="29" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C29" s="12">
         <v>14</v>
       </c>
-      <c r="D29" s="42"/>
+      <c r="D29" s="42" t="s">
+        <v>82</v>
+      </c>
       <c r="E29" s="42"/>
       <c r="F29" s="42"/>
       <c r="G29" s="42"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="33"/>
+      <c r="H29" s="32">
+        <v>7</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="32">
+        <v>3</v>
+      </c>
+      <c r="K29" s="32">
+        <v>2</v>
+      </c>
+      <c r="L29" s="33">
+        <v>0.99999999999870004</v>
+      </c>
       <c r="M29" s="32"/>
       <c r="N29" s="32"/>
       <c r="T29" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>ISBLANK(D29)</f>
+        <v>0</v>
       </c>
       <c r="U29" s="2">
         <v>13</v>
@@ -8208,24 +8549,36 @@
         <v>0.13541666666666699</v>
       </c>
     </row>
-    <row r="30" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C30" s="13">
         <v>15</v>
       </c>
-      <c r="D30" s="39"/>
+      <c r="D30" s="39" t="s">
+        <v>83</v>
+      </c>
       <c r="E30" s="39"/>
       <c r="F30" s="39"/>
       <c r="G30" s="39"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="35"/>
+      <c r="H30" s="34">
+        <v>29</v>
+      </c>
+      <c r="I30" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="34">
+        <v>3</v>
+      </c>
+      <c r="K30" s="34">
+        <v>3</v>
+      </c>
+      <c r="L30" s="35">
+        <v>0.83333333333307302</v>
+      </c>
       <c r="M30" s="34"/>
       <c r="N30" s="34"/>
       <c r="T30" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>ISBLANK(D30)</f>
+        <v>0</v>
       </c>
       <c r="U30" s="2">
         <v>14</v>
@@ -8240,24 +8593,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C31" s="12">
         <v>16</v>
       </c>
-      <c r="D31" s="42"/>
+      <c r="D31" s="42" t="s">
+        <v>84</v>
+      </c>
       <c r="E31" s="42"/>
       <c r="F31" s="42"/>
       <c r="G31" s="42"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="33"/>
+      <c r="H31" s="32">
+        <v>30</v>
+      </c>
+      <c r="I31" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="32">
+        <v>1</v>
+      </c>
+      <c r="K31" s="32">
+        <v>1</v>
+      </c>
+      <c r="L31" s="33">
+        <v>0.250000000000003</v>
+      </c>
       <c r="M31" s="32"/>
       <c r="N31" s="32"/>
       <c r="T31" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>ISBLANK(D31)</f>
+        <v>0</v>
       </c>
       <c r="U31" s="2">
         <v>15</v>
@@ -8270,31 +8635,43 @@
       </c>
       <c r="AD31" s="1">
         <f>COUNTIF(Categorie,AC31)</f>
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="AE31" s="19">
         <f>SUMIFS(Duree, Categorie,AC31)</f>
-        <v>1.3229166666653667</v>
-      </c>
-    </row>
-    <row r="32" spans="3:31" x14ac:dyDescent="0.3">
+        <v>6.4062499999970894</v>
+      </c>
+    </row>
+    <row r="32" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C32" s="13">
         <v>17</v>
       </c>
-      <c r="D32" s="39"/>
+      <c r="D32" s="39" t="s">
+        <v>85</v>
+      </c>
       <c r="E32" s="39"/>
       <c r="F32" s="39"/>
       <c r="G32" s="39"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="35"/>
+      <c r="H32" s="34">
+        <v>29</v>
+      </c>
+      <c r="I32" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="34">
+        <v>1</v>
+      </c>
+      <c r="K32" s="34">
+        <v>1</v>
+      </c>
+      <c r="L32" s="35">
+        <v>0.416666666666696</v>
+      </c>
       <c r="M32" s="34"/>
       <c r="N32" s="34"/>
       <c r="T32" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>ISBLANK(D32)</f>
+        <v>0</v>
       </c>
       <c r="U32" s="2">
         <v>16</v>
@@ -8307,31 +8684,43 @@
       </c>
       <c r="AD32" s="1">
         <f>COUNTIF(Categorie,AC32)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE32" s="19">
         <f>SUMIFS(Duree, Categorie,AC32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:31" x14ac:dyDescent="0.3">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="33" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C33" s="12">
         <v>18</v>
       </c>
-      <c r="D33" s="42"/>
+      <c r="D33" s="42" t="s">
+        <v>86</v>
+      </c>
       <c r="E33" s="42"/>
       <c r="F33" s="42"/>
       <c r="G33" s="42"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="33"/>
+      <c r="H33" s="32">
+        <v>29</v>
+      </c>
+      <c r="I33" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="32">
+        <v>1</v>
+      </c>
+      <c r="K33" s="32">
+        <v>1</v>
+      </c>
+      <c r="L33" s="33">
+        <v>0.416666666666696</v>
+      </c>
       <c r="M33" s="32"/>
       <c r="N33" s="32"/>
       <c r="T33" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>ISBLANK(D33)</f>
+        <v>0</v>
       </c>
       <c r="U33" s="2">
         <v>17</v>
@@ -8351,24 +8740,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C34" s="13">
         <v>19</v>
       </c>
-      <c r="D34" s="39"/>
+      <c r="D34" s="39" t="s">
+        <v>87</v>
+      </c>
       <c r="E34" s="39"/>
       <c r="F34" s="39"/>
       <c r="G34" s="39"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="35"/>
+      <c r="H34" s="34">
+        <v>30</v>
+      </c>
+      <c r="I34" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="34">
+        <v>2</v>
+      </c>
+      <c r="K34" s="34">
+        <v>3</v>
+      </c>
+      <c r="L34" s="35">
+        <v>0.62499999999988298</v>
+      </c>
       <c r="M34" s="34"/>
       <c r="N34" s="34"/>
       <c r="T34" s="1" t="b">
         <f>ISBLANK(D34)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U34" s="2">
         <v>18</v>
@@ -8377,11 +8778,13 @@
         <v>0.187499999999998</v>
       </c>
     </row>
-    <row r="35" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C35" s="12">
         <v>20</v>
       </c>
-      <c r="D35" s="42"/>
+      <c r="D35" s="42" t="s">
+        <v>88</v>
+      </c>
       <c r="E35" s="42"/>
       <c r="F35" s="42"/>
       <c r="G35" s="42"/>
@@ -8393,8 +8796,8 @@
       <c r="M35" s="32"/>
       <c r="N35" s="32"/>
       <c r="T35" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>ISBLANK(D35)</f>
+        <v>0</v>
       </c>
       <c r="U35" s="2">
         <v>19</v>
@@ -8409,11 +8812,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C36" s="13">
         <v>21</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="39" t="s">
+        <v>89</v>
+      </c>
       <c r="E36" s="39"/>
       <c r="F36" s="39"/>
       <c r="G36" s="39"/>
@@ -8426,7 +8831,7 @@
       <c r="N36" s="34"/>
       <c r="T36" s="1" t="b">
         <f>ISBLANK(D36)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U36" s="2">
         <v>20</v>
@@ -8439,18 +8844,20 @@
       </c>
       <c r="AD36" s="1">
         <f>COUNTIF(Difficulte,W17)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="AE36" s="19">
         <f>SUMIFS(Duree, Difficulte,W17)</f>
-        <v>7.2916666666666671E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="3:31" x14ac:dyDescent="0.3">
+        <v>1.6979166666667314</v>
+      </c>
+    </row>
+    <row r="37" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C37" s="12">
         <v>22</v>
       </c>
-      <c r="D37" s="42"/>
+      <c r="D37" s="42" t="s">
+        <v>102</v>
+      </c>
       <c r="E37" s="42"/>
       <c r="F37" s="42"/>
       <c r="G37" s="42"/>
@@ -8463,7 +8870,7 @@
       <c r="N37" s="32"/>
       <c r="T37" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U37" s="2">
         <v>21</v>
@@ -8476,18 +8883,20 @@
       </c>
       <c r="AD37" s="1">
         <f>COUNTIF(Difficulte,W18)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AE37" s="19">
         <f>SUMIFS(Duree, Difficulte,W18)</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="38" spans="3:31" x14ac:dyDescent="0.3">
+        <v>1.2083333333332149</v>
+      </c>
+    </row>
+    <row r="38" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C38" s="13">
         <v>23</v>
       </c>
-      <c r="D38" s="39"/>
+      <c r="D38" s="39" t="s">
+        <v>90</v>
+      </c>
       <c r="E38" s="39"/>
       <c r="F38" s="39"/>
       <c r="G38" s="39"/>
@@ -8500,7 +8909,7 @@
       <c r="N38" s="34"/>
       <c r="T38" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U38" s="2">
         <v>22</v>
@@ -8513,18 +8922,20 @@
       </c>
       <c r="AD38" s="1">
         <f>COUNTIF(Difficulte,W19)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AE38" s="19">
         <f>SUMIFS(Duree, Difficulte,W19)</f>
-        <v>0.99999999999870004</v>
-      </c>
-    </row>
-    <row r="39" spans="3:31" x14ac:dyDescent="0.3">
+        <v>3.7083333333304758</v>
+      </c>
+    </row>
+    <row r="39" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C39" s="12">
         <v>24</v>
       </c>
-      <c r="D39" s="42"/>
+      <c r="D39" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="E39" s="42"/>
       <c r="F39" s="42"/>
       <c r="G39" s="42"/>
@@ -8537,7 +8948,7 @@
       <c r="N39" s="32"/>
       <c r="T39" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U39" s="2">
         <v>23</v>
@@ -8546,11 +8957,13 @@
         <v>0.27083333333333998</v>
       </c>
     </row>
-    <row r="40" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C40" s="13">
         <v>25</v>
       </c>
-      <c r="D40" s="39"/>
+      <c r="D40" s="39" t="s">
+        <v>92</v>
+      </c>
       <c r="E40" s="39"/>
       <c r="F40" s="39"/>
       <c r="G40" s="39"/>
@@ -8563,7 +8976,7 @@
       <c r="N40" s="34"/>
       <c r="T40" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U40" s="2">
         <v>24</v>
@@ -8578,11 +8991,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C41" s="12">
         <v>26</v>
       </c>
-      <c r="D41" s="42"/>
+      <c r="D41" s="42" t="s">
+        <v>95</v>
+      </c>
       <c r="E41" s="42"/>
       <c r="F41" s="42"/>
       <c r="G41" s="42"/>
@@ -8595,7 +9010,7 @@
       <c r="N41" s="32"/>
       <c r="T41" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U41" s="2">
         <v>25</v>
@@ -8608,18 +9023,20 @@
       </c>
       <c r="AD41" s="1">
         <f>COUNTIF(Incertitude,X17)</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="AE41" s="19">
         <f>SUMIFS(Duree, Incertitude,X17)</f>
-        <v>0.32291666666666669</v>
-      </c>
-    </row>
-    <row r="42" spans="3:31" x14ac:dyDescent="0.3">
+        <v>2.2812500000000635</v>
+      </c>
+    </row>
+    <row r="42" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C42" s="13">
         <v>27</v>
       </c>
-      <c r="D42" s="39"/>
+      <c r="D42" s="39" t="s">
+        <v>94</v>
+      </c>
       <c r="E42" s="39"/>
       <c r="F42" s="39"/>
       <c r="G42" s="39"/>
@@ -8632,7 +9049,7 @@
       <c r="N42" s="34"/>
       <c r="T42" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U42" s="2">
         <v>26</v>
@@ -8645,18 +9062,20 @@
       </c>
       <c r="AD42" s="1">
         <f>COUNTIF(Incertitude,X18)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AE42" s="19">
         <f>SUMIFS(Duree, Incertitude,X18)</f>
-        <v>0.99999999999870004</v>
-      </c>
-    </row>
-    <row r="43" spans="3:31" x14ac:dyDescent="0.3">
+        <v>2.874999999997403</v>
+      </c>
+    </row>
+    <row r="43" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C43" s="12">
         <v>28</v>
       </c>
-      <c r="D43" s="42"/>
+      <c r="D43" s="42" t="s">
+        <v>93</v>
+      </c>
       <c r="E43" s="42"/>
       <c r="F43" s="42"/>
       <c r="G43" s="42"/>
@@ -8669,7 +9088,7 @@
       <c r="N43" s="32"/>
       <c r="T43" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U43" s="2">
         <v>27</v>
@@ -8682,18 +9101,20 @@
       </c>
       <c r="AD43" s="1">
         <f>COUNTIF(Incertitude,X19)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE43" s="19">
         <f>SUMIFS(Duree, Incertitude,X19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="3:31" x14ac:dyDescent="0.3">
+        <v>1.458333333332956</v>
+      </c>
+    </row>
+    <row r="44" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C44" s="13">
         <v>29</v>
       </c>
-      <c r="D44" s="39"/>
+      <c r="D44" s="39" t="s">
+        <v>96</v>
+      </c>
       <c r="E44" s="39"/>
       <c r="F44" s="39"/>
       <c r="G44" s="39"/>
@@ -8706,7 +9127,7 @@
       <c r="N44" s="34"/>
       <c r="T44" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U44" s="2">
         <v>28</v>
@@ -8715,11 +9136,13 @@
         <v>0.37500000000002298</v>
       </c>
     </row>
-    <row r="45" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C45" s="12">
         <v>30</v>
       </c>
-      <c r="D45" s="42"/>
+      <c r="D45" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="E45" s="42"/>
       <c r="F45" s="42"/>
       <c r="G45" s="42"/>
@@ -8732,7 +9155,7 @@
       <c r="N45" s="32"/>
       <c r="T45" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U45" s="2">
         <v>29</v>
@@ -8741,11 +9164,13 @@
         <v>0.39583333333336002</v>
       </c>
     </row>
-    <row r="46" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C46" s="13">
         <v>31</v>
       </c>
-      <c r="D46" s="39"/>
+      <c r="D46" s="39" t="s">
+        <v>98</v>
+      </c>
       <c r="E46" s="39"/>
       <c r="F46" s="39"/>
       <c r="G46" s="39"/>
@@ -8758,7 +9183,7 @@
       <c r="N46" s="34"/>
       <c r="T46" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U46" s="2">
         <v>30</v>
@@ -8767,11 +9192,13 @@
         <v>0.416666666666696</v>
       </c>
     </row>
-    <row r="47" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C47" s="12">
         <v>32</v>
       </c>
-      <c r="D47" s="42"/>
+      <c r="D47" s="42" t="s">
+        <v>99</v>
+      </c>
       <c r="E47" s="42"/>
       <c r="F47" s="42"/>
       <c r="G47" s="42"/>
@@ -8784,7 +9211,7 @@
       <c r="N47" s="32"/>
       <c r="T47" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U47" s="2">
         <v>31</v>
@@ -8793,11 +9220,13 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="48" spans="3:31" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:31" x14ac:dyDescent="0.15">
       <c r="C48" s="13">
         <v>33</v>
       </c>
-      <c r="D48" s="39"/>
+      <c r="D48" s="39" t="s">
+        <v>101</v>
+      </c>
       <c r="E48" s="39"/>
       <c r="F48" s="39"/>
       <c r="G48" s="39"/>
@@ -8810,7 +9239,7 @@
       <c r="N48" s="34"/>
       <c r="T48" s="1" t="b">
         <f t="shared" ref="T48:T65" si="4">ISBLANK(D48)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U48" s="2">
         <v>32</v>
@@ -8819,11 +9248,13 @@
         <v>0.49999999999997102</v>
       </c>
     </row>
-    <row r="49" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C49" s="12">
         <v>34</v>
       </c>
-      <c r="D49" s="42"/>
+      <c r="D49" s="42" t="s">
+        <v>103</v>
+      </c>
       <c r="E49" s="42"/>
       <c r="F49" s="42"/>
       <c r="G49" s="42"/>
@@ -8836,7 +9267,7 @@
       <c r="N49" s="32"/>
       <c r="T49" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U49" s="2">
         <v>33</v>
@@ -8848,11 +9279,13 @@
         <v>0.54166666666660801</v>
       </c>
     </row>
-    <row r="50" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C50" s="13">
         <v>35</v>
       </c>
-      <c r="D50" s="39"/>
+      <c r="D50" s="39" t="s">
+        <v>104</v>
+      </c>
       <c r="E50" s="39"/>
       <c r="F50" s="39"/>
       <c r="G50" s="39"/>
@@ -8865,7 +9298,7 @@
       <c r="N50" s="34"/>
       <c r="T50" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U50" s="2">
         <v>34</v>
@@ -8877,11 +9310,13 @@
         <v>0.583333333333245</v>
       </c>
     </row>
-    <row r="51" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C51" s="12">
         <v>36</v>
       </c>
-      <c r="D51" s="42"/>
+      <c r="D51" s="42" t="s">
+        <v>100</v>
+      </c>
       <c r="E51" s="42"/>
       <c r="F51" s="42"/>
       <c r="G51" s="42"/>
@@ -8893,8 +9328,8 @@
       <c r="M51" s="32"/>
       <c r="N51" s="32"/>
       <c r="T51" s="1" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>ISBLANK(D51)</f>
+        <v>0</v>
       </c>
       <c r="U51" s="2">
         <v>35</v>
@@ -8906,11 +9341,13 @@
         <v>0.62499999999988298</v>
       </c>
     </row>
-    <row r="52" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C52" s="13">
         <v>37</v>
       </c>
-      <c r="D52" s="39"/>
+      <c r="D52" s="39" t="s">
+        <v>105</v>
+      </c>
       <c r="E52" s="39"/>
       <c r="F52" s="39"/>
       <c r="G52" s="39"/>
@@ -8922,8 +9359,8 @@
       <c r="M52" s="34"/>
       <c r="N52" s="34"/>
       <c r="T52" s="1" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>ISBLANK(D52)</f>
+        <v>0</v>
       </c>
       <c r="U52" s="2">
         <v>36</v>
@@ -8935,7 +9372,7 @@
         <v>0.66666666666652097</v>
       </c>
     </row>
-    <row r="53" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C53" s="12">
         <v>38</v>
       </c>
@@ -8964,7 +9401,7 @@
         <v>0.70833333333315895</v>
       </c>
     </row>
-    <row r="54" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C54" s="13">
         <v>39</v>
       </c>
@@ -8993,7 +9430,7 @@
         <v>0.74999999999979705</v>
       </c>
     </row>
-    <row r="55" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C55" s="12">
         <v>40</v>
       </c>
@@ -9022,7 +9459,7 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="56" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C56" s="13">
         <v>41</v>
       </c>
@@ -9051,7 +9488,7 @@
         <v>0.83333333333307302</v>
       </c>
     </row>
-    <row r="57" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C57" s="12">
         <v>42</v>
       </c>
@@ -9080,7 +9517,7 @@
         <v>0.87499999999947897</v>
       </c>
     </row>
-    <row r="58" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C58" s="13">
         <v>43</v>
       </c>
@@ -9109,7 +9546,7 @@
         <v>0.91666666666588603</v>
       </c>
     </row>
-    <row r="59" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C59" s="12">
         <v>44</v>
       </c>
@@ -9138,7 +9575,7 @@
         <v>0.95833333333229298</v>
       </c>
     </row>
-    <row r="60" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C60" s="13">
         <v>45</v>
       </c>
@@ -9167,7 +9604,7 @@
         <v>0.99999999999870004</v>
       </c>
     </row>
-    <row r="61" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C61" s="12">
         <v>46</v>
       </c>
@@ -9196,7 +9633,7 @@
         <v>1.04166666666511</v>
       </c>
     </row>
-    <row r="62" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C62" s="13">
         <v>47</v>
       </c>
@@ -9225,7 +9662,7 @@
         <v>1.0833333333315101</v>
       </c>
     </row>
-    <row r="63" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C63" s="12">
         <v>48</v>
       </c>
@@ -9254,7 +9691,7 @@
         <v>1.1249999999979201</v>
       </c>
     </row>
-    <row r="64" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C64" s="13">
         <v>49</v>
       </c>
@@ -9283,7 +9720,7 @@
         <v>1.1666666666643299</v>
       </c>
     </row>
-    <row r="65" spans="3:25" s="1" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:25" s="1" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C65" s="14">
         <v>50</v>
       </c>
@@ -9312,7 +9749,7 @@
         <v>1.20833333333073</v>
       </c>
     </row>
-    <row r="66" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
@@ -9327,7 +9764,7 @@
         <v>1.2499999999971401</v>
       </c>
     </row>
-    <row r="67" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
@@ -9340,10 +9777,10 @@
       <c r="X67" s="2"/>
       <c r="Y67" s="9"/>
     </row>
-    <row r="68" spans="3:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="D68" s="1">
         <f>COUNTA(D16:D65)</f>
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -9351,7 +9788,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="9">
         <f>SUM(L16:L65)</f>
-        <v>1.3229166666653667</v>
+        <v>6.6145833333304225</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -9362,7 +9799,7 @@
         <v>1.2916666666635499</v>
       </c>
     </row>
-    <row r="69" spans="3:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
@@ -9377,7 +9814,7 @@
         <v>1.33333333332996</v>
       </c>
     </row>
-    <row r="70" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
@@ -9392,7 +9829,7 @@
         <v>1.37499999999636</v>
       </c>
     </row>
-    <row r="71" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
@@ -9407,7 +9844,7 @@
         <v>1.4166666666627701</v>
       </c>
     </row>
-    <row r="72" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
@@ -9422,7 +9859,7 @@
         <v>1.4583333333291799</v>
       </c>
     </row>
-    <row r="73" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
@@ -9437,7 +9874,7 @@
         <v>1.49999999999558</v>
       </c>
     </row>
-    <row r="74" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
@@ -9452,7 +9889,7 @@
         <v>1.54166666666199</v>
       </c>
     </row>
-    <row r="75" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
@@ -9467,7 +9904,7 @@
         <v>1.5833333333284001</v>
       </c>
     </row>
-    <row r="76" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
@@ -9482,7 +9919,7 @@
         <v>1.6249999999948099</v>
       </c>
     </row>
-    <row r="77" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
@@ -9497,7 +9934,7 @@
         <v>1.66666666666121</v>
       </c>
     </row>
-    <row r="78" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
@@ -9512,7 +9949,7 @@
         <v>1.7083333333276201</v>
       </c>
     </row>
-    <row r="79" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
@@ -9527,7 +9964,7 @@
         <v>1.7499999999940301</v>
       </c>
     </row>
-    <row r="80" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
@@ -9542,87 +9979,87 @@
         <v>1.79166666666043</v>
       </c>
     </row>
-    <row r="81" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y81" s="9">
         <v>1.83333333332684</v>
       </c>
     </row>
-    <row r="82" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y82" s="9">
         <v>1.8749999999932501</v>
       </c>
     </row>
-    <row r="83" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y83" s="9">
         <v>1.9166666666596599</v>
       </c>
     </row>
-    <row r="84" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y84" s="9">
         <v>1.95833333332606</v>
       </c>
     </row>
-    <row r="85" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y85" s="9">
         <v>1.99999999999247</v>
       </c>
     </row>
-    <row r="86" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y86" s="9">
         <v>2.0416666666588701</v>
       </c>
     </row>
-    <row r="87" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y87" s="9">
         <v>2.0833333333252799</v>
       </c>
     </row>
-    <row r="88" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y88" s="9">
         <v>2.1249999999916902</v>
       </c>
     </row>
-    <row r="89" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y89" s="9">
         <v>2.1666666666580898</v>
       </c>
     </row>
-    <row r="90" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y90" s="9">
         <v>2.2083333333245001</v>
       </c>
     </row>
-    <row r="91" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y91" s="9">
         <v>2.2499999999909099</v>
       </c>
     </row>
-    <row r="92" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y92" s="9">
         <v>2.2916666666573202</v>
       </c>
     </row>
-    <row r="93" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y93" s="9">
         <v>2.3333333333237198</v>
       </c>
     </row>
-    <row r="94" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y94" s="9">
         <v>2.3749999999901301</v>
       </c>
     </row>
-    <row r="95" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y95" s="9">
         <v>2.41666666665654</v>
       </c>
     </row>
-    <row r="96" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y96" s="9">
         <v>2.45833333332294</v>
       </c>
     </row>
-    <row r="97" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="25:25" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="Y97" s="9">
         <v>2.4999999999893499</v>
       </c>
@@ -9630,6 +10067,7 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="tjqSiT+XspradLJBNpu0viI4TokIDIF0O7QeXm3BTZLmeAfSOw5TlniSFfStQ9LXJLtK7gLyf3B6jINr+qJ+Cg==" saltValue="/wSmyHkNAfBsPbW8NILu1w==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="56">
+    <mergeCell ref="D35:G35"/>
     <mergeCell ref="D63:G63"/>
     <mergeCell ref="D64:G64"/>
     <mergeCell ref="D65:G65"/>
@@ -9657,9 +10095,6 @@
     <mergeCell ref="D49:G49"/>
     <mergeCell ref="D50:G50"/>
     <mergeCell ref="D44:G44"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="D35:G35"/>
     <mergeCell ref="D36:G36"/>
     <mergeCell ref="D37:G37"/>
     <mergeCell ref="D38:G38"/>
@@ -9680,6 +10115,8 @@
     <mergeCell ref="D29:G29"/>
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="D33:G33"/>
     <mergeCell ref="D20:G20"/>
     <mergeCell ref="D15:G15"/>
     <mergeCell ref="D16:G16"/>
@@ -9802,14 +10239,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:13" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="46" t="s">
         <v>36</v>
       </c>
@@ -9819,8 +10256,8 @@
       <c r="F2" s="46"/>
       <c r="G2" s="46"/>
     </row>
-    <row r="3" spans="2:13" ht="10.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:13" ht="10.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="22"/>
       <c r="C4" s="22" t="s">
         <v>13</v>
@@ -9838,7 +10275,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="s">
         <v>31</v>
       </c>
@@ -9863,7 +10300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="21" t="s">
         <v>20</v>
       </c>
@@ -9888,7 +10325,7 @@
         <v>1.3229166666653667</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="48" t="s">
         <v>51</v>
       </c>
@@ -9904,7 +10341,7 @@
       <c r="L9" s="48"/>
       <c r="M9" s="48"/>
     </row>
-    <row r="10" spans="2:13" ht="10.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="2:13" ht="10.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="7jx2YjRECZ6o8Bp/12l6CT33ZUxVZFIE8DruIq28qeqGO2CO/14nabG1jCRVqb35hCSmvSIufKDGdWZOjYPEuQ==" saltValue="Nt1swAwRwjrWuMUX30XPfw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="2">
@@ -9924,14 +10361,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="2.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="1" max="4" width="2.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="48" t="s">
         <v>37</v>
       </c>
@@ -9952,150 +10389,150 @@
       <c r="Q2" s="48"/>
       <c r="R2" s="48"/>
     </row>
-    <row r="3" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="4" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="C4" s="23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:18" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D5" s="24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="2:18" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D6" s="24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:18" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="D7" s="24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:18" s="1" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="2:18" s="1" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="2:18" s="1" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" s="1" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D10" s="24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:18" s="1" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" s="1" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D11" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="2:18" s="1" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" s="1" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D12" s="27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D13" s="24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D14" s="24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D15" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D16" s="24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D17" s="24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D18" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="20" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="C22" s="23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D23" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D24" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D25" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D26" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D27" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D28" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:5" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="E29" s="24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:5" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="E30" s="24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="E31" s="24" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D32" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="34" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="35" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="36" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="37" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="38" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="39" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="40" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="41" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="42" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="43" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="44" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="45" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="46" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="33" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="34" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="35" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="36" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="37" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="38" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="39" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="40" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="41" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="42" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="43" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="44" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="45" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
+    <row r="46" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Dzyfz6Pvoe1+wPoVjXKJsRTFywgjIP8eSEZi7eXOnUCA2h3K3cNX0zQIho1YSjNBBIX99v4/FYUmXsSWPOGxxw==" saltValue="B5CvoY9Z3hcMlbc34txcfw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
docs: filled the document_planification.xlms
</commit_message>
<xml_diff>
--- a/docs/EnCours/Sprint1c - Outil de planification.xlsx
+++ b/docs/EnCours/Sprint1c - Outil de planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julienc./Desktop/KitchenCompanion/docs/EnCours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99A37C0-10DF-1545-AA44-242F9A37E3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8C6BF2-3D42-F14E-9D38-BE62BD3A134C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="24900" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planification" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -264,7 +264,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -273,15 +273,61 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Il existe 3 catégories de tâche :
- - Essentielle | tâche obligatoire devant être réalisée
- - Souhaitable | tâche envisagée sérieusement
- - Optionnelle | tâche facultative selon l'évolution du projet</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Il existe 3 catégories de tâche :
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - Essentielle | tâche obligatoire devant être réalisée
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - Souhaitable | tâche envisagée sérieusement
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - Optionnelle | tâche facultative selon l'évolution du projet</t>
         </r>
       </text>
     </comment>
@@ -364,7 +410,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -375,7 +421,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -384,12 +430,31 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Délai de développement estimé pour réaliser la tâche.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Délai de développement estimé pour réaliser la tâche.</t>
         </r>
       </text>
     </comment>
@@ -469,7 +534,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="109">
   <si>
     <t>Planification</t>
   </si>
@@ -916,6 +981,12 @@
   </si>
   <si>
     <t>00.15</t>
+  </si>
+  <si>
+    <t>JC</t>
+  </si>
+  <si>
+    <t>RC</t>
   </si>
 </sst>
 </file>
@@ -1805,13 +1876,13 @@
                   <c:v>1.3229166666653667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.666666666665173</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.6666666666665653</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.4166666666666363</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2208,10 +2279,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.666666666665173</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2325,10 +2396,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.6666666666665653</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2444,10 +2515,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.4166666666666363</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2780,10 +2851,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>18</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4062499999970894</c:v>
+                  <c:v>7.4479166666637715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2839,10 +2910,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20833333333333334</c:v>
+                  <c:v>1.5833333333333919</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2898,10 +2969,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.0416666666665781</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3233,10 +3304,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6979166666667314</c:v>
+                  <c:v>3.1979166666667207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3292,10 +3363,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2083333333332149</c:v>
+                  <c:v>3.1249999999999658</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3351,10 +3422,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7083333333304758</c:v>
+                  <c:v>4.7499999999970548</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3686,10 +3757,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>13</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2812500000000635</c:v>
+                  <c:v>3.7812500000000528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3745,10 +3816,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.874999999997403</c:v>
+                  <c:v>3.9583333333307622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3804,10 +3875,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.458333333332956</c:v>
+                  <c:v>3.3333333333329267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7579,8 +7650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AF97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C16" zoomScale="178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="178" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -7754,7 +7825,7 @@
       <c r="N13" s="46"/>
       <c r="U13" s="2">
         <f>D68</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA13" s="2">
         <f>N7</f>
@@ -7997,11 +8068,11 @@
       </c>
       <c r="AD18" s="1">
         <f>COUNTIF(Sprint,AC18)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AE18" s="19">
         <f>SUMIFS(Duree, Sprint,AC18)</f>
-        <v>0</v>
+        <v>4.666666666665173</v>
       </c>
     </row>
     <row r="19" spans="3:31" x14ac:dyDescent="0.15">
@@ -8070,11 +8141,11 @@
       </c>
       <c r="AD19" s="1">
         <f>COUNTIF(Sprint,AC19)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AE19" s="19">
         <f>SUMIFS(Duree, Sprint,AC19)</f>
-        <v>0</v>
+        <v>1.6666666666665653</v>
       </c>
     </row>
     <row r="20" spans="3:31" x14ac:dyDescent="0.15">
@@ -8102,8 +8173,12 @@
       <c r="L20" s="35">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
+      <c r="M20" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T20" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8127,11 +8202,11 @@
       </c>
       <c r="AD20" s="1">
         <f>COUNTIF(Sprint,AC20)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AE20" s="19">
         <f>SUMIFS(Duree, Sprint,AC20)</f>
-        <v>0</v>
+        <v>3.4166666666666363</v>
       </c>
     </row>
     <row r="21" spans="3:31" x14ac:dyDescent="0.15">
@@ -8159,8 +8234,12 @@
       <c r="L21" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
+      <c r="M21" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" s="32" t="s">
+        <v>107</v>
+      </c>
       <c r="T21" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8201,8 +8280,12 @@
       <c r="L22" s="35">
         <v>0.16666666666666599</v>
       </c>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
+      <c r="M22" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" s="34" t="s">
+        <v>108</v>
+      </c>
       <c r="T22" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8239,8 +8322,12 @@
       <c r="L23" s="33">
         <v>0.16666666666666599</v>
       </c>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
+      <c r="M23" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N23" s="32" t="s">
+        <v>108</v>
+      </c>
       <c r="T23" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8286,8 +8373,12 @@
       <c r="L24" s="35">
         <v>0.250000000000003</v>
       </c>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
+      <c r="M24" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" s="34" t="s">
+        <v>107</v>
+      </c>
       <c r="T24" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8304,11 +8395,11 @@
       </c>
       <c r="AD24" s="1">
         <f>COUNTIF(Responsabilite,AC24)</f>
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="AE24" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC24)</f>
-        <v>1.3229166666653667</v>
+        <v>7.2812499999969722</v>
       </c>
     </row>
     <row r="25" spans="3:31" x14ac:dyDescent="0.15">
@@ -8336,8 +8427,12 @@
       <c r="L25" s="33">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
+      <c r="M25" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N25" s="32" t="s">
+        <v>107</v>
+      </c>
       <c r="T25" s="1" t="b">
         <f>ISBLANK(D25)</f>
         <v>0</v>
@@ -8354,11 +8449,11 @@
       </c>
       <c r="AD25" s="1">
         <f>COUNTIF(Responsabilite,AC25)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AE25" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC25)</f>
-        <v>0</v>
+        <v>1.7916666666667314</v>
       </c>
     </row>
     <row r="26" spans="3:31" x14ac:dyDescent="0.15">
@@ -8386,8 +8481,12 @@
       <c r="L26" s="35">
         <v>0.625</v>
       </c>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
+      <c r="M26" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N26" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T26" s="1" t="b">
         <f>ISBLANK(D26)</f>
         <v>0</v>
@@ -8404,11 +8503,11 @@
       </c>
       <c r="AD26" s="1">
         <f>COUNTIF(Responsabilite,AC26)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AE26" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC26)</f>
-        <v>0</v>
+        <v>2.0000000000000395</v>
       </c>
     </row>
     <row r="27" spans="3:31" x14ac:dyDescent="0.15">
@@ -8436,8 +8535,12 @@
       <c r="L27" s="33">
         <v>0.20833333333333334</v>
       </c>
-      <c r="M27" s="32"/>
-      <c r="N27" s="32"/>
+      <c r="M27" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N27" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T27" s="1" t="b">
         <f>ISBLANK(D27)</f>
         <v>0</v>
@@ -8454,11 +8557,11 @@
       </c>
       <c r="AD27" s="1">
         <f>COUNTIF(Responsabilite,AC27)</f>
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="AE27" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC27)</f>
-        <v>5.2916666666650558</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="3:31" x14ac:dyDescent="0.15">
@@ -8486,8 +8589,12 @@
       <c r="L28" s="35">
         <v>0.250000000000003</v>
       </c>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
+      <c r="M28" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" s="34" t="s">
+        <v>107</v>
+      </c>
       <c r="T28" s="1" t="b">
         <f>ISBLANK(D28)</f>
         <v>0</v>
@@ -8504,11 +8611,11 @@
       </c>
       <c r="AD28" s="1">
         <f>COUNTIF(Responsabilite,AC28)</f>
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="AE28" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC28)</f>
-        <v>5.2916666666650558</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="3:31" x14ac:dyDescent="0.15">
@@ -8536,8 +8643,12 @@
       <c r="L29" s="33">
         <v>0.99999999999870004</v>
       </c>
-      <c r="M29" s="32"/>
-      <c r="N29" s="32"/>
+      <c r="M29" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T29" s="1" t="b">
         <f>ISBLANK(D29)</f>
         <v>0</v>
@@ -8560,7 +8671,7 @@
       <c r="F30" s="39"/>
       <c r="G30" s="39"/>
       <c r="H30" s="34">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="I30" s="34" t="s">
         <v>17</v>
@@ -8574,8 +8685,12 @@
       <c r="L30" s="35">
         <v>0.83333333333307302</v>
       </c>
-      <c r="M30" s="34"/>
-      <c r="N30" s="34"/>
+      <c r="M30" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N30" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T30" s="1" t="b">
         <f>ISBLANK(D30)</f>
         <v>0</v>
@@ -8604,7 +8719,7 @@
       <c r="F31" s="42"/>
       <c r="G31" s="42"/>
       <c r="H31" s="32">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I31" s="32" t="s">
         <v>17</v>
@@ -8618,8 +8733,12 @@
       <c r="L31" s="33">
         <v>0.250000000000003</v>
       </c>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
+      <c r="M31" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N31" s="32" t="s">
+        <v>108</v>
+      </c>
       <c r="T31" s="1" t="b">
         <f>ISBLANK(D31)</f>
         <v>0</v>
@@ -8635,11 +8754,11 @@
       </c>
       <c r="AD31" s="1">
         <f>COUNTIF(Categorie,AC31)</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="AE31" s="19">
         <f>SUMIFS(Duree, Categorie,AC31)</f>
-        <v>6.4062499999970894</v>
+        <v>7.4479166666637715</v>
       </c>
     </row>
     <row r="32" spans="3:31" x14ac:dyDescent="0.15">
@@ -8653,7 +8772,7 @@
       <c r="F32" s="39"/>
       <c r="G32" s="39"/>
       <c r="H32" s="34">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="I32" s="34" t="s">
         <v>17</v>
@@ -8667,8 +8786,12 @@
       <c r="L32" s="35">
         <v>0.416666666666696</v>
       </c>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
+      <c r="M32" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N32" s="34" t="s">
+        <v>107</v>
+      </c>
       <c r="T32" s="1" t="b">
         <f>ISBLANK(D32)</f>
         <v>0</v>
@@ -8684,11 +8807,11 @@
       </c>
       <c r="AD32" s="1">
         <f>COUNTIF(Categorie,AC32)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AE32" s="19">
         <f>SUMIFS(Duree, Categorie,AC32)</f>
-        <v>0.20833333333333334</v>
+        <v>1.5833333333333919</v>
       </c>
     </row>
     <row r="33" spans="3:31" x14ac:dyDescent="0.15">
@@ -8702,7 +8825,7 @@
       <c r="F33" s="42"/>
       <c r="G33" s="42"/>
       <c r="H33" s="32">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="I33" s="32" t="s">
         <v>17</v>
@@ -8716,8 +8839,12 @@
       <c r="L33" s="33">
         <v>0.416666666666696</v>
       </c>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
+      <c r="M33" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N33" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T33" s="1" t="b">
         <f>ISBLANK(D33)</f>
         <v>0</v>
@@ -8733,11 +8860,11 @@
       </c>
       <c r="AD33" s="1">
         <f>COUNTIF(Categorie,AC33)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE33" s="19">
         <f>SUMIFS(Duree, Categorie,AC33)</f>
-        <v>0</v>
+        <v>2.0416666666665781</v>
       </c>
     </row>
     <row r="34" spans="3:31" x14ac:dyDescent="0.15">
@@ -8751,7 +8878,7 @@
       <c r="F34" s="39"/>
       <c r="G34" s="39"/>
       <c r="H34" s="34">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I34" s="34" t="s">
         <v>17</v>
@@ -8765,8 +8892,12 @@
       <c r="L34" s="35">
         <v>0.62499999999988298</v>
       </c>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34"/>
+      <c r="M34" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N34" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T34" s="1" t="b">
         <f>ISBLANK(D34)</f>
         <v>0</v>
@@ -8788,13 +8919,27 @@
       <c r="E35" s="42"/>
       <c r="F35" s="42"/>
       <c r="G35" s="42"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
+      <c r="H35" s="32">
+        <v>9</v>
+      </c>
+      <c r="I35" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="32">
+        <v>1</v>
+      </c>
+      <c r="K35" s="32">
+        <v>1</v>
+      </c>
+      <c r="L35" s="33">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="M35" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N35" s="32" t="s">
+        <v>107</v>
+      </c>
       <c r="T35" s="1" t="b">
         <f>ISBLANK(D35)</f>
         <v>0</v>
@@ -8822,13 +8967,27 @@
       <c r="E36" s="39"/>
       <c r="F36" s="39"/>
       <c r="G36" s="39"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
+      <c r="H36" s="34">
+        <v>7</v>
+      </c>
+      <c r="I36" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="34">
+        <v>2</v>
+      </c>
+      <c r="K36" s="34">
+        <v>2</v>
+      </c>
+      <c r="L36" s="35">
+        <v>0.33333333333335002</v>
+      </c>
+      <c r="M36" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N36" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T36" s="1" t="b">
         <f>ISBLANK(D36)</f>
         <v>0</v>
@@ -8844,11 +9003,11 @@
       </c>
       <c r="AD36" s="1">
         <f>COUNTIF(Difficulte,W17)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AE36" s="19">
         <f>SUMIFS(Duree, Difficulte,W17)</f>
-        <v>1.6979166666667314</v>
+        <v>3.1979166666667207</v>
       </c>
     </row>
     <row r="37" spans="3:31" x14ac:dyDescent="0.15">
@@ -8861,13 +9020,27 @@
       <c r="E37" s="42"/>
       <c r="F37" s="42"/>
       <c r="G37" s="42"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
+      <c r="H37" s="32">
+        <v>21</v>
+      </c>
+      <c r="I37" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="32">
+        <v>1</v>
+      </c>
+      <c r="K37" s="32">
+        <v>1</v>
+      </c>
+      <c r="L37" s="33">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="M37" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N37" s="32" t="s">
+        <v>108</v>
+      </c>
       <c r="T37" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8883,11 +9056,11 @@
       </c>
       <c r="AD37" s="1">
         <f>COUNTIF(Difficulte,W18)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="AE37" s="19">
         <f>SUMIFS(Duree, Difficulte,W18)</f>
-        <v>1.2083333333332149</v>
+        <v>3.1249999999999658</v>
       </c>
     </row>
     <row r="38" spans="3:31" x14ac:dyDescent="0.15">
@@ -8900,13 +9073,27 @@
       <c r="E38" s="39"/>
       <c r="F38" s="39"/>
       <c r="G38" s="39"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="34"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
+      <c r="H38" s="34">
+        <v>21</v>
+      </c>
+      <c r="I38" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="34">
+        <v>2</v>
+      </c>
+      <c r="K38" s="34">
+        <v>2</v>
+      </c>
+      <c r="L38" s="35">
+        <v>0.250000000000003</v>
+      </c>
+      <c r="M38" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N38" s="34" t="s">
+        <v>108</v>
+      </c>
       <c r="T38" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8922,11 +9109,11 @@
       </c>
       <c r="AD38" s="1">
         <f>COUNTIF(Difficulte,W19)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AE38" s="19">
         <f>SUMIFS(Duree, Difficulte,W19)</f>
-        <v>3.7083333333304758</v>
+        <v>4.7499999999970548</v>
       </c>
     </row>
     <row r="39" spans="3:31" x14ac:dyDescent="0.15">
@@ -8934,18 +9121,32 @@
         <v>24</v>
       </c>
       <c r="D39" s="42" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="E39" s="42"/>
       <c r="F39" s="42"/>
       <c r="G39" s="42"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
+      <c r="H39" s="32">
+        <v>9</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="32">
+        <v>1</v>
+      </c>
+      <c r="K39" s="32">
+        <v>1</v>
+      </c>
+      <c r="L39" s="33">
+        <v>0.20833333333333001</v>
+      </c>
+      <c r="M39" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N39" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T39" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8962,18 +9163,32 @@
         <v>25</v>
       </c>
       <c r="D40" s="39" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E40" s="39"/>
       <c r="F40" s="39"/>
       <c r="G40" s="39"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
-      <c r="K40" s="34"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="34"/>
-      <c r="N40" s="34"/>
+      <c r="H40" s="34">
+        <v>7</v>
+      </c>
+      <c r="I40" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J40" s="34">
+        <v>1</v>
+      </c>
+      <c r="K40" s="34">
+        <v>1</v>
+      </c>
+      <c r="L40" s="35">
+        <v>0.20833333333333001</v>
+      </c>
+      <c r="M40" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N40" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T40" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8996,18 +9211,32 @@
         <v>26</v>
       </c>
       <c r="D41" s="42" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E41" s="42"/>
       <c r="F41" s="42"/>
       <c r="G41" s="42"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
+      <c r="H41" s="32">
+        <v>25</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" s="32">
+        <v>1</v>
+      </c>
+      <c r="K41" s="32">
+        <v>1</v>
+      </c>
+      <c r="L41" s="33">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="M41" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="32" t="s">
+        <v>107</v>
+      </c>
       <c r="T41" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9023,11 +9252,11 @@
       </c>
       <c r="AD41" s="1">
         <f>COUNTIF(Incertitude,X17)</f>
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="AE41" s="19">
         <f>SUMIFS(Duree, Incertitude,X17)</f>
-        <v>2.2812500000000635</v>
+        <v>3.7812500000000528</v>
       </c>
     </row>
     <row r="42" spans="3:31" x14ac:dyDescent="0.15">
@@ -9035,18 +9264,32 @@
         <v>27</v>
       </c>
       <c r="D42" s="39" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E42" s="39"/>
       <c r="F42" s="39"/>
       <c r="G42" s="39"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
+      <c r="H42" s="34">
+        <v>25</v>
+      </c>
+      <c r="I42" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J42" s="34">
+        <v>1</v>
+      </c>
+      <c r="K42" s="34">
+        <v>1</v>
+      </c>
+      <c r="L42" s="35">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="M42" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N42" s="34" t="s">
+        <v>107</v>
+      </c>
       <c r="T42" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9062,11 +9305,11 @@
       </c>
       <c r="AD42" s="1">
         <f>COUNTIF(Incertitude,X18)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AE42" s="19">
         <f>SUMIFS(Duree, Incertitude,X18)</f>
-        <v>2.874999999997403</v>
+        <v>3.9583333333307622</v>
       </c>
     </row>
     <row r="43" spans="3:31" x14ac:dyDescent="0.15">
@@ -9074,18 +9317,32 @@
         <v>28</v>
       </c>
       <c r="D43" s="42" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E43" s="42"/>
       <c r="F43" s="42"/>
       <c r="G43" s="42"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="33"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
+      <c r="H43" s="32">
+        <v>25</v>
+      </c>
+      <c r="I43" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" s="32">
+        <v>2</v>
+      </c>
+      <c r="K43" s="32">
+        <v>2</v>
+      </c>
+      <c r="L43" s="33">
+        <v>0.250000000000003</v>
+      </c>
+      <c r="M43" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N43" s="32" t="s">
+        <v>108</v>
+      </c>
       <c r="T43" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9101,11 +9358,11 @@
       </c>
       <c r="AD43" s="1">
         <f>COUNTIF(Incertitude,X19)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AE43" s="19">
         <f>SUMIFS(Duree, Incertitude,X19)</f>
-        <v>1.458333333332956</v>
+        <v>3.3333333333329267</v>
       </c>
     </row>
     <row r="44" spans="3:31" x14ac:dyDescent="0.15">
@@ -9113,18 +9370,32 @@
         <v>29</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E44" s="39"/>
       <c r="F44" s="39"/>
       <c r="G44" s="39"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
-      <c r="K44" s="34"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="34"/>
-      <c r="N44" s="34"/>
+      <c r="H44" s="34">
+        <v>18</v>
+      </c>
+      <c r="I44" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="J44" s="34">
+        <v>2</v>
+      </c>
+      <c r="K44" s="34">
+        <v>2</v>
+      </c>
+      <c r="L44" s="35">
+        <v>0.250000000000003</v>
+      </c>
+      <c r="M44" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N44" s="34" t="s">
+        <v>108</v>
+      </c>
       <c r="T44" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9141,18 +9412,32 @@
         <v>30</v>
       </c>
       <c r="D45" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E45" s="42"/>
       <c r="F45" s="42"/>
       <c r="G45" s="42"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="33"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32"/>
+      <c r="H45" s="32">
+        <v>7</v>
+      </c>
+      <c r="I45" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="J45" s="32">
+        <v>1</v>
+      </c>
+      <c r="K45" s="32">
+        <v>1</v>
+      </c>
+      <c r="L45" s="33">
+        <v>0.20833333333333001</v>
+      </c>
+      <c r="M45" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N45" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T45" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9169,18 +9454,32 @@
         <v>31</v>
       </c>
       <c r="D46" s="39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E46" s="39"/>
       <c r="F46" s="39"/>
       <c r="G46" s="39"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="34"/>
-      <c r="N46" s="34"/>
+      <c r="H46" s="34">
+        <v>3</v>
+      </c>
+      <c r="I46" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="J46" s="34">
+        <v>2</v>
+      </c>
+      <c r="K46" s="34">
+        <v>3</v>
+      </c>
+      <c r="L46" s="35">
+        <v>0.416666666666696</v>
+      </c>
+      <c r="M46" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N46" s="34" t="s">
+        <v>108</v>
+      </c>
       <c r="T46" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9197,18 +9496,32 @@
         <v>32</v>
       </c>
       <c r="D47" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E47" s="42"/>
       <c r="F47" s="42"/>
       <c r="G47" s="42"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="33"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32"/>
+      <c r="H47" s="32">
+        <v>31</v>
+      </c>
+      <c r="I47" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="J47" s="32">
+        <v>1</v>
+      </c>
+      <c r="K47" s="32">
+        <v>1</v>
+      </c>
+      <c r="L47" s="33">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="M47" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N47" s="32" t="s">
+        <v>108</v>
+      </c>
       <c r="T47" s="1" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9225,18 +9538,32 @@
         <v>33</v>
       </c>
       <c r="D48" s="39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E48" s="39"/>
       <c r="F48" s="39"/>
       <c r="G48" s="39"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="34"/>
-      <c r="K48" s="34"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="34"/>
-      <c r="N48" s="34"/>
+      <c r="H48" s="34">
+        <v>7</v>
+      </c>
+      <c r="I48" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J48" s="34">
+        <v>1</v>
+      </c>
+      <c r="K48" s="34">
+        <v>1</v>
+      </c>
+      <c r="L48" s="35">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="M48" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N48" s="34" t="s">
+        <v>107</v>
+      </c>
       <c r="T48" s="1" t="b">
         <f t="shared" ref="T48:T65" si="4">ISBLANK(D48)</f>
         <v>0</v>
@@ -9253,18 +9580,32 @@
         <v>34</v>
       </c>
       <c r="D49" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E49" s="42"/>
       <c r="F49" s="42"/>
       <c r="G49" s="42"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="33"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="32"/>
+      <c r="H49" s="32">
+        <v>9</v>
+      </c>
+      <c r="I49" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J49" s="32">
+        <v>1</v>
+      </c>
+      <c r="K49" s="32">
+        <v>1</v>
+      </c>
+      <c r="L49" s="33">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="M49" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N49" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T49" s="1" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -9284,18 +9625,32 @@
         <v>35</v>
       </c>
       <c r="D50" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E50" s="39"/>
       <c r="F50" s="39"/>
       <c r="G50" s="39"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="34"/>
-      <c r="L50" s="35"/>
-      <c r="M50" s="34"/>
-      <c r="N50" s="34"/>
+      <c r="H50" s="34">
+        <v>7</v>
+      </c>
+      <c r="I50" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J50" s="34">
+        <v>2</v>
+      </c>
+      <c r="K50" s="34">
+        <v>3</v>
+      </c>
+      <c r="L50" s="35">
+        <v>0.416666666666696</v>
+      </c>
+      <c r="M50" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N50" s="34" t="s">
+        <v>107</v>
+      </c>
       <c r="T50" s="1" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -9315,18 +9670,32 @@
         <v>36</v>
       </c>
       <c r="D51" s="42" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E51" s="42"/>
       <c r="F51" s="42"/>
       <c r="G51" s="42"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="33"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
+      <c r="H51" s="32">
+        <v>16</v>
+      </c>
+      <c r="I51" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J51" s="32">
+        <v>3</v>
+      </c>
+      <c r="K51" s="32">
+        <v>3</v>
+      </c>
+      <c r="L51" s="33">
+        <v>0.62499999999988298</v>
+      </c>
+      <c r="M51" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N51" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T51" s="1" t="b">
         <f>ISBLANK(D51)</f>
         <v>0</v>
@@ -9346,18 +9715,32 @@
         <v>37</v>
       </c>
       <c r="D52" s="39" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E52" s="39"/>
       <c r="F52" s="39"/>
       <c r="G52" s="39"/>
-      <c r="H52" s="34"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="34"/>
-      <c r="K52" s="34"/>
-      <c r="L52" s="35"/>
-      <c r="M52" s="34"/>
-      <c r="N52" s="34"/>
+      <c r="H52" s="34">
+        <v>6</v>
+      </c>
+      <c r="I52" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="J52" s="34">
+        <v>3</v>
+      </c>
+      <c r="K52" s="34">
+        <v>3</v>
+      </c>
+      <c r="L52" s="35">
+        <v>0.416666666666696</v>
+      </c>
+      <c r="M52" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N52" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T52" s="1" t="b">
         <f>ISBLANK(D52)</f>
         <v>0</v>
@@ -9376,7 +9759,9 @@
       <c r="C53" s="12">
         <v>38</v>
       </c>
-      <c r="D53" s="42"/>
+      <c r="D53" s="42" t="s">
+        <v>105</v>
+      </c>
       <c r="E53" s="42"/>
       <c r="F53" s="42"/>
       <c r="G53" s="42"/>
@@ -9389,7 +9774,7 @@
       <c r="N53" s="32"/>
       <c r="T53" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U53" s="2">
         <v>37</v>
@@ -9780,7 +10165,7 @@
     <row r="68" spans="3:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="D68" s="1">
         <f>COUNTA(D16:D65)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -9788,7 +10173,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="9">
         <f>SUM(L16:L65)</f>
-        <v>6.6145833333304225</v>
+        <v>11.072916666663744</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -10285,19 +10670,19 @@
       </c>
       <c r="D5" s="8">
         <f>COUNTIF(Sprint,D4)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E5" s="8">
         <f>COUNTIF(Sprint,E4)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F5" s="8">
         <f>COUNTIF(Sprint,F4)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G5" s="25">
         <f>SUM(C5:F5)</f>
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
@@ -10310,19 +10695,19 @@
       </c>
       <c r="D6" s="10">
         <f>SUMIFS(Duree, Sprint,D4)</f>
-        <v>0</v>
+        <v>4.666666666665173</v>
       </c>
       <c r="E6" s="10">
         <f>SUMIFS(Duree, Sprint,E4)</f>
-        <v>0</v>
+        <v>1.6666666666665653</v>
       </c>
       <c r="F6" s="10">
         <f>SUMIFS(Duree, Sprint,F4)</f>
-        <v>0</v>
+        <v>3.4166666666666363</v>
       </c>
       <c r="G6" s="26">
         <f>SUM(C6:F6)</f>
-        <v>1.3229166666653667</v>
+        <v>11.07291666666374</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>